<commit_message>
realizadas las pruebas funcionales
</commit_message>
<xml_diff>
--- a/Pruebas funcionales.xlsx
+++ b/Pruebas funcionales.xlsx
@@ -1,23 +1,181 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76708E5-B2EA-43CD-AFF2-94B18040E4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Prueba 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Prueba 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Prueba 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+  <si>
+    <t>VALIDACION</t>
+  </si>
+  <si>
+    <t>NOMBRE DEL CASO</t>
+  </si>
+  <si>
+    <t>DESCRIPCION</t>
+  </si>
+  <si>
+    <t>PASOS</t>
+  </si>
+  <si>
+    <t>RESULTADO ESPERADO</t>
+  </si>
+  <si>
+    <t>RESULTADO REAL</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
+  </si>
+  <si>
+    <t>RESPONSABLE</t>
+  </si>
+  <si>
+    <t>COMENTARIOS</t>
+  </si>
+  <si>
+    <t>ejecucion main.ts</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Octavio Mastrangelo</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>validar entrada incorrecta del menu</t>
+  </si>
+  <si>
+    <t>verificar que el programa detecte y maneje opciones de entradas no validas correctamente</t>
+  </si>
+  <si>
+    <t>1 - ejecutar el programa 2 - mostrar el menu principal 3 - ingresar uina opcion no valida, por ejemplo "3"</t>
+  </si>
+  <si>
+    <t>El sistema muestra un mensaje de error indicando "Ingreso una opción incorrecta, intente nuevamente</t>
+  </si>
+  <si>
+    <t>El sistema muestra "Ingreso una opción incorrecta, intente nuevamente" y vuelve a mostrar el menú principal.</t>
+  </si>
+  <si>
+    <t>Ignacio Galardo</t>
+  </si>
+  <si>
+    <t>validar rango de apuestas en ruleta</t>
+  </si>
+  <si>
+    <t>Verificar que el sistema detecte y maneje apuestas fuera del rango permitido (0 a 36).</t>
+  </si>
+  <si>
+    <t>Seleccionar la opción "1, Ruleta".
+Ingresar un número fuera del rango permitido, como 37.
+Repetir con otro número fuera del rango, como -1.
+Intentar hasta que el sistema pida ingresar un número válido.</t>
+  </si>
+  <si>
+    <t>El sistema muestra el mensaje "Ingreso un número incorrecto, vuelva a ingresar" y vuelve a pedir una apuesta válida.</t>
+  </si>
+  <si>
+    <t>El sistema muestra "Ingreso un número incorrecto, vuelva a ingresar" y sigue pidiendo un número válido. Pasó</t>
+  </si>
+  <si>
+    <t>Juan Bintana</t>
+  </si>
+  <si>
+    <t>Alexis Ullmann</t>
+  </si>
+  <si>
+    <t>Validar perdida en tragamonedas 3x3</t>
+  </si>
+  <si>
+    <t>Verificar que el sistema actualice correctamente el saldo del jugador al perder una apuesta en tragamonedas.</t>
+  </si>
+  <si>
+    <t>1. Apostar 500 créditos.
+Activar la tragamonedas.
+Observar el resultado (sin combinaciones ganadoras).
+Confirmar actualización del saldo.</t>
+  </si>
+  <si>
+    <t>El sistema muestra el mensaje "Lo lamentamos. Perdiste", resta los créditos apostados del saldo y actualiza el saldo correctamente</t>
+  </si>
+  <si>
+    <t>El sistema muestra "Lo lamentamos. Perdiste", resta los créditos correctamente y actualiza el saldo a 49000 créditos.</t>
+  </si>
+  <si>
+    <t>Verificar que el sistema procese correctamente múltiples tiradas automáticas en tragamonedas con apuestas fuertes.</t>
+  </si>
+  <si>
+    <t>Ingresar a la opción "3, Tragamonedas (5x3 Lineas)".
+Seleccionar tiradas automáticas (opción 2).
+Ingresar cantidad de tiradas: 5.
+Ingresar cantidad a apostar: 2000.
+Verificar que cada tirada reste correctamente la apuesta y actualice el saldo hasta que finalicen las tiradas.</t>
+  </si>
+  <si>
+    <t>El sistema realiza 5 tiradas automáticas, muestra los resultados, resta 2000 por tirada del saldo, y actualiza correctamente el saldo final.</t>
+  </si>
+  <si>
+    <t>El sistema realiza 5 tiradas automáticas, resta correctamente 2000 por tirada, actualiza el saldo y muestra los resultados de cada tirada.</t>
+  </si>
+  <si>
+    <t>validar tiradas automaticas tragamonedas 3x3</t>
+  </si>
+  <si>
+    <t>Nadia Mujica</t>
+  </si>
+  <si>
+    <t>validar apuesta y ganancia en carrera</t>
+  </si>
+  <si>
+    <t>Verificar que el sistema maneje correctamente las apuestas en carreras de caballos y calcule las ganancias al ganar.</t>
+  </si>
+  <si>
+    <t>Apostar 39000 créditos al caballo N° 12.
+Iniciar la carrera.
+Verificar que el sistema determine correctamente si el caballo gana.
+Confirmar que las ganancias se calculen y actualicen correctamente en el saldo.</t>
+  </si>
+  <si>
+    <t>El sistema muestra un mensaje de victoria y calcula la ganancia total (39000 x multiplicador de ganancia). El saldo se actualiza correctamente.</t>
+  </si>
+  <si>
+    <t>El sistema muestra "Felicidades tu caballo es el ganador!!", calcula correctamente 351000 de ganancia y actualiza el saldo.</t>
+  </si>
+  <si>
+    <t>verificar que el programa se inicie sin errores</t>
+  </si>
+  <si>
+    <t>1 - se inicia la consola 2 - se ejecuta el archivo main.ts</t>
+  </si>
+  <si>
+    <t>El sistema funciona correctamente, mostrando el menu principal sin problemas.</t>
+  </si>
+  <si>
+    <t>El sistema funciona sin errores, mostrando el menu principal del sistema</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -25,16 +183,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -42,25 +239,141 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF99FF66"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Oficina">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -98,9 +411,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Oficina">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -132,9 +445,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -166,9 +497,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Oficina">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -341,25 +690,242 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="40.81640625" customWidth="1"/>
+    <col min="4" max="4" width="45.26953125" customWidth="1"/>
+    <col min="5" max="5" width="42.08984375" customWidth="1"/>
+    <col min="6" max="6" width="42.81640625" customWidth="1"/>
+    <col min="8" max="8" width="13.90625" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="11">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A4" s="11">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="11">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -367,14 +933,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9951CD41-6416-4CD7-A855-1A1E1B855A9E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>